<commit_message>
Added six test cases for Radio Buttons
</commit_message>
<xml_diff>
--- a/TestCases/ZavrsniProjekat.xlsx
+++ b/TestCases/ZavrsniProjekat.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="271">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -843,30 +843,56 @@
     <t xml:space="preserve">The prompt box disappears from screen and text doesn’t appear</t>
   </si>
   <si>
-    <t xml:space="preserve">Scenario CheckBox</t>
+    <t xml:space="preserve">Scenario Radio Button</t>
   </si>
   <si>
     <t xml:space="preserve">TC_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the “Radio Button” page is opened when a user clicks on “Radio Button tab” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the “Radio Button” tab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The “Radio Button” page is loaded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that all elements are present and visible on the Radio Button page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the sentence “Do you like the site?” is present above radio buttons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sentence “Do you like the site?” is present above radio buttons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check radio buttons: “Yes” , “Impressive” , “No” are present and visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The radio buttons: “Yes” , “Impressive” and “No” are present and visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that when a user clicks on the “Yes” radio button, the button is selected, and a text “You have selected Yes” appears underneath the radio buttons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No radio button is selected</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Verify that when the user clicks on “Check Box” a new page “</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Check Box</t>
+      <t xml:space="preserve">Click on “</t>
     </r>
     <r>
       <rPr>
@@ -876,14 +902,231 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">” is opened.</t>
+      <t xml:space="preserve">Yes</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on the “Check Box” tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The “Check Box” page loaded , Header of Page is “Check Box”</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” radio button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The radio button “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Yes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” is selected and text appears “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You have selected Yes”</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that when a user clicks on the “Impressive” radio button, the button is selected, and a text “You have selected Impressive” appears underneath the radio buttons.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Click on “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Impressive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” radio button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The radio button “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Impressive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” is selected and text appears “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You have selected Impressive”</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that when a user can’t click the radio button “No” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on “No” radio button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mouse pointer transforms into a restricted sign and the radio button can't be clicked.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that a user can switch between radio buttons.Only one radio button can be selected</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The radio button “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Impressive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” is selected and text appears “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You have selected Impressive” and the “Yes” radio button is deselected</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The radio button did not switch, the radio button “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Impressive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” is selected and text appears “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">You have selected Impressive”</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Url:</t>
@@ -1065,7 +1308,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1107,12 +1350,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1195,7 +1432,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1284,6 +1521,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1324,7 +1565,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1417,12 +1658,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F199"/>
+  <dimension ref="A1:F233"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D205" activeCellId="0" sqref="D205"/>
+      <selection pane="bottomLeft" activeCell="D239" activeCellId="0" sqref="D239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3865,62 +4106,484 @@
       <c r="E195" s="5"/>
       <c r="F195" s="5"/>
     </row>
-    <row r="196" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="6" t="s">
         <v>187</v>
       </c>
       <c r="B196" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C196" s="7"/>
+      <c r="C196" s="20"/>
       <c r="D196" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E196" s="7"/>
-      <c r="F196" s="7" t="s">
+      <c r="E196" s="20"/>
+      <c r="F196" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="6"/>
-      <c r="B197" s="7"/>
-      <c r="C197" s="7"/>
+      <c r="A197" s="20"/>
+      <c r="B197" s="15"/>
+      <c r="C197" s="20"/>
       <c r="D197" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F197" s="7" t="s">
+      <c r="F197" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="6"/>
-      <c r="B198" s="7"/>
-      <c r="C198" s="7"/>
+      <c r="A198" s="20"/>
+      <c r="B198" s="20"/>
+      <c r="C198" s="20"/>
       <c r="D198" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E198" s="18"/>
+      <c r="E198" s="20"/>
       <c r="F198" s="9" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="6"/>
-      <c r="B199" s="7"/>
-      <c r="C199" s="7"/>
+      <c r="A199" s="20"/>
+      <c r="B199" s="20"/>
+      <c r="C199" s="20"/>
       <c r="D199" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E199" s="7"/>
+      <c r="E199" s="20"/>
       <c r="F199" s="9" t="s">
         <v>190</v>
       </c>
     </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="5"/>
+      <c r="B200" s="5"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+      <c r="E200" s="5"/>
+      <c r="F200" s="5"/>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B201" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C201" s="0"/>
+      <c r="D201" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E201" s="20"/>
+      <c r="F201" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="20"/>
+      <c r="B202" s="15"/>
+      <c r="C202" s="0"/>
+      <c r="D202" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E202" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F202" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="20"/>
+      <c r="B203" s="20"/>
+      <c r="C203" s="0"/>
+      <c r="D203" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E203" s="20"/>
+      <c r="F203" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="20"/>
+      <c r="B204" s="20"/>
+      <c r="C204" s="20"/>
+      <c r="D204" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E204" s="20"/>
+      <c r="F204" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="20"/>
+      <c r="B205" s="20"/>
+      <c r="C205" s="20"/>
+      <c r="D205" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E205" s="20"/>
+      <c r="F205" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="20"/>
+      <c r="B206" s="20"/>
+      <c r="C206" s="20"/>
+      <c r="D206" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E206" s="20"/>
+      <c r="F206" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="5"/>
+      <c r="B207" s="5"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
+      <c r="F207" s="5"/>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A208" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B208" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C208" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D208" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E208" s="20"/>
+      <c r="F208" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="20"/>
+      <c r="B209" s="15"/>
+      <c r="C209" s="11"/>
+      <c r="D209" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F209" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="20"/>
+      <c r="B210" s="15"/>
+      <c r="C210" s="11"/>
+      <c r="D210" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E210" s="20"/>
+      <c r="F210" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="20"/>
+      <c r="B211" s="20"/>
+      <c r="C211" s="20"/>
+      <c r="D211" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E211" s="20"/>
+      <c r="F211" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="20"/>
+      <c r="B212" s="20"/>
+      <c r="C212" s="20"/>
+      <c r="D212" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E212" s="20"/>
+      <c r="F212" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="5"/>
+      <c r="B213" s="5"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+      <c r="E213" s="5"/>
+      <c r="F213" s="5"/>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A214" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B214" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C214" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D214" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E214" s="20"/>
+      <c r="F214" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="20"/>
+      <c r="B215" s="15"/>
+      <c r="C215" s="11"/>
+      <c r="D215" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F215" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="20"/>
+      <c r="B216" s="15"/>
+      <c r="C216" s="11"/>
+      <c r="D216" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E216" s="20"/>
+      <c r="F216" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="20"/>
+      <c r="B217" s="20"/>
+      <c r="C217" s="20"/>
+      <c r="D217" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E217" s="20"/>
+      <c r="F217" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="20"/>
+      <c r="B218" s="20"/>
+      <c r="C218" s="20"/>
+      <c r="D218" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E218" s="20"/>
+      <c r="F218" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="5"/>
+      <c r="B219" s="5"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="5"/>
+      <c r="E219" s="5"/>
+      <c r="F219" s="5"/>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A220" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B220" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C220" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D220" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E220" s="20"/>
+      <c r="F220" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="20"/>
+      <c r="B221" s="15"/>
+      <c r="C221" s="11"/>
+      <c r="D221" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E221" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F221" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="20"/>
+      <c r="B222" s="15"/>
+      <c r="C222" s="11"/>
+      <c r="D222" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E222" s="20"/>
+      <c r="F222" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="20"/>
+      <c r="B223" s="20"/>
+      <c r="C223" s="20"/>
+      <c r="D223" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E223" s="20"/>
+      <c r="F223" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="20"/>
+      <c r="B224" s="20"/>
+      <c r="C224" s="20"/>
+      <c r="D224" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E224" s="20"/>
+      <c r="F224" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="5"/>
+      <c r="B225" s="5"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="5"/>
+      <c r="E225" s="5"/>
+      <c r="F225" s="5"/>
+    </row>
+    <row r="226" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A226" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B226" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C226" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D226" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E226" s="20"/>
+      <c r="F226" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="20"/>
+      <c r="B227" s="15"/>
+      <c r="C227" s="11"/>
+      <c r="D227" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F227" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="20"/>
+      <c r="B228" s="15"/>
+      <c r="C228" s="11"/>
+      <c r="D228" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E228" s="20"/>
+      <c r="F228" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="20"/>
+      <c r="B229" s="20"/>
+      <c r="C229" s="20"/>
+      <c r="D229" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E229" s="20"/>
+      <c r="F229" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="20"/>
+      <c r="B230" s="20"/>
+      <c r="C230" s="20"/>
+      <c r="D230" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E230" s="20"/>
+      <c r="F230" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="20"/>
+      <c r="B231" s="20"/>
+      <c r="C231" s="20"/>
+      <c r="D231" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E231" s="20"/>
+      <c r="F231" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="20"/>
+      <c r="B232" s="20"/>
+      <c r="C232" s="20"/>
+      <c r="D232" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E232" s="20"/>
+      <c r="F232" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="5"/>
+      <c r="B233" s="5"/>
+      <c r="C233" s="5"/>
+      <c r="D233" s="5"/>
+      <c r="E233" s="5"/>
+      <c r="F233" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="61">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B15:B16"/>
@@ -3969,6 +4632,19 @@
     <mergeCell ref="A187:F187"/>
     <mergeCell ref="B188:B190"/>
     <mergeCell ref="A195:F195"/>
+    <mergeCell ref="B196:B197"/>
+    <mergeCell ref="A200:F200"/>
+    <mergeCell ref="A207:F207"/>
+    <mergeCell ref="B208:B210"/>
+    <mergeCell ref="C208:C210"/>
+    <mergeCell ref="A213:F213"/>
+    <mergeCell ref="B214:B216"/>
+    <mergeCell ref="C214:C216"/>
+    <mergeCell ref="A219:F219"/>
+    <mergeCell ref="C220:C222"/>
+    <mergeCell ref="A225:F225"/>
+    <mergeCell ref="C226:C228"/>
+    <mergeCell ref="A233:F233"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="https://demoqa.com/"/>
@@ -4015,6 +4691,11 @@
     <hyperlink ref="E181" r:id="rId42" display="https://demoqa.com/"/>
     <hyperlink ref="E189" r:id="rId43" display="https://demoqa.com/"/>
     <hyperlink ref="E197" r:id="rId44" display="https://demoqa.com/"/>
+    <hyperlink ref="E202" r:id="rId45" display="https://demoqa.com/"/>
+    <hyperlink ref="E209" r:id="rId46" display="https://demoqa.com/"/>
+    <hyperlink ref="E215" r:id="rId47" display="https://demoqa.com/"/>
+    <hyperlink ref="E221" r:id="rId48" display="https://demoqa.com/"/>
+    <hyperlink ref="E227" r:id="rId49" display="https://demoqa.com/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4039,9 +4720,9 @@
       <selection pane="bottomLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="64.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="54.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="34.78"/>
@@ -4049,7 +4730,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
@@ -4059,205 +4740,205 @@
     </row>
     <row r="2" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>193</v>
+        <v>215</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="B5" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="7" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28" t="s">
-        <v>201</v>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29" t="s">
+        <v>224</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="B11" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="2" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="D12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="B13" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27"/>
-      <c r="B14" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>207</v>
+      <c r="A14" s="28"/>
+      <c r="B14" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>230</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="B15" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27"/>
-      <c r="B16" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>208</v>
+      <c r="A16" s="28"/>
+      <c r="B16" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>231</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27"/>
-      <c r="B18" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>210</v>
+      <c r="A18" s="28"/>
+      <c r="B18" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>233</v>
       </c>
       <c r="D18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="B19" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="28" t="s">
-        <v>212</v>
+      <c r="B20" s="29" t="s">
+        <v>235</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="D20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="B21" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="D22" s="7"/>
     </row>
@@ -4266,7 +4947,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="D23" s="7"/>
     </row>
@@ -4275,7 +4956,7 @@
         <v>65</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="D24" s="7"/>
     </row>
@@ -4284,278 +4965,278 @@
         <v>65</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="D25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="B26" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="D27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="D28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
+      <c r="B29" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>222</v>
+      <c r="B30" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="B31" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
+      <c r="B33" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="B35" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="B35" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
-      <c r="B36" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>227</v>
+      <c r="B36" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B38" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
+      <c r="B38" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>229</v>
+      <c r="B39" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B40" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="B40" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B42" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
+      <c r="B42" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="B44" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
+      <c r="B44" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
+      <c r="B46" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="B48" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="B50" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="29" t="s">
-        <v>241</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>241</v>
+      <c r="B51" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="B52" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
+      <c r="B52" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="33" t="s">
-        <v>243</v>
+      <c r="C53" s="34" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B54" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
+      <c r="B54" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4593,34 +5274,34 @@
       <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>193</v>
+        <v>215</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>216</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20"/>
@@ -4704,8 +5385,8 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
-      <c r="B13" s="35" t="s">
-        <v>247</v>
+      <c r="B13" s="36" t="s">
+        <v>270</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>

</xml_diff>

<commit_message>
Tested Radio Button Page
</commit_message>
<xml_diff>
--- a/TestCases/ZavrsniProjekat.xlsx
+++ b/TestCases/ZavrsniProjekat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="279">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -1288,10 +1288,34 @@
     <t xml:space="preserve">You entered Vlada</t>
   </si>
   <si>
-    <t xml:space="preserve">Header of Chech Box page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Box</t>
+    <t xml:space="preserve">Header of RadioButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radio Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elements Of RadioButtonPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you like the site?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impressive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text Selected Yes Radio Button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have selected Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have selected Impressive</t>
   </si>
   <si>
     <t xml:space="preserve">Invalid Email Address</t>
@@ -1308,7 +1332,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1357,6 +1381,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1432,7 +1461,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1573,6 +1602,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1660,10 +1693,10 @@
   </sheetPr>
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D239" activeCellId="0" sqref="D239"/>
+      <selection pane="bottomLeft" activeCell="C241" activeCellId="0" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4712,15 +4745,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+      <selection pane="bottomLeft" activeCell="B76" activeCellId="0" sqref="B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="64.19"/>
@@ -5237,6 +5270,84 @@
       </c>
       <c r="C55" s="2" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -5274,7 +5385,7 @@
       <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.08"/>
   </cols>
@@ -5283,7 +5394,7 @@
       <c r="A1" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>216</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -5298,7 +5409,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -5385,8 +5496,8 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
-      <c r="B13" s="36" t="s">
-        <v>270</v>
+      <c r="B13" s="37" t="s">
+        <v>278</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>

</xml_diff>